<commit_message>
Refatorar código para seguir convenções de nomenclatura e estilo
</commit_message>
<xml_diff>
--- a/Scripts/cliniclaudio_Dr Claudio/Agendamentos.xlsx
+++ b/Scripts/cliniclaudio_Dr Claudio/Agendamentos.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8aa611cfd27d87da/Documentos/testeImportacao/Scripts/cliniclaudio_Dr Claudio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_7C1511AFD3C0D6A7B42907D04B5ED87656CD5617" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FD22105-FF65-4697-B38B-6D7D6EC2DCB4}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_7C1511AFD320DFE7502905D04B5ED87656CD5617" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9915F05-ACB8-4102-9D97-CF31E6592FB9}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$89</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -653,12 +656,19 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -689,48 +699,48 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2">
-        <v>44936.385416666657</v>
+        <v>45096.6875</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
-        <v>44941.583333333343</v>
+        <v>45236.645833333343</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
@@ -741,80 +751,80 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="2">
-        <v>44946.489583333343</v>
+        <v>45336.572916666657</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2">
-        <v>44951.6875</v>
+        <v>44962.541666666657</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2">
-        <v>44956.427083333343</v>
+        <v>45166.677083333343</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -828,123 +838,123 @@
         <v>21</v>
       </c>
       <c r="D7" s="2">
-        <v>44962.541666666657</v>
+        <v>45276.583333333343</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44941.583333333343</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2">
-        <v>44967.40625</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
-        <v>44972.5</v>
+        <v>45101.385416666657</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2">
-        <v>44977.645833333343</v>
+        <v>45241.375</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2">
-        <v>44982.458333333343</v>
+        <v>44986.677083333343</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -955,172 +965,172 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2">
-        <v>44986.677083333343</v>
+        <v>45201.375</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2">
-        <v>44991.395833333343</v>
+        <v>45311.489583333343</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="2">
-        <v>44996.53125</v>
+        <v>44936.385416666657</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2">
-        <v>45001.583333333343</v>
+        <v>45171.489583333343</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2">
-        <v>45006.4375</v>
+        <v>45296.645833333343</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2">
-        <v>45011.697916666657</v>
+        <v>44991.395833333343</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
         <v>29</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2">
-        <v>45016.385416666657</v>
+        <v>45141.385416666657</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -1131,51 +1141,51 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2">
-        <v>45021.458333333343</v>
+        <v>45256.583333333343</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="2">
-        <v>45026.572916666657</v>
+        <v>44951.6875</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H20" t="s">
         <v>30</v>
@@ -1183,152 +1193,152 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="2">
-        <v>45031.645833333343</v>
+        <v>45121.375</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2">
-        <v>45036.375</v>
+        <v>45246.677083333343</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2">
-        <v>45041.677083333343</v>
+        <v>45051.583333333343</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="2">
-        <v>45046.489583333343</v>
+        <v>45211.489583333343</v>
       </c>
       <c r="E24" t="s">
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
         <v>18</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2">
-        <v>45051.583333333343</v>
+        <v>44972.5</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D26" s="2">
-        <v>45056.395833333343</v>
+        <v>45106.458333333343</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
@@ -1339,77 +1349,77 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D27" s="2">
-        <v>45061.697916666657</v>
+        <v>45266.6875</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2">
-        <v>45066.427083333343</v>
+        <v>45011.697916666657</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="2">
-        <v>45071.541666666657</v>
+        <v>45146.458333333343</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H29" t="s">
         <v>25</v>
@@ -1417,337 +1427,337 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D30" s="2">
-        <v>45076.65625</v>
+        <v>45056.395833333343</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
         <v>18</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D31" s="2">
-        <v>45081.375</v>
+        <v>45151.572916666657</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H31" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D32" s="2">
-        <v>45086.46875</v>
+        <v>45306.677083333343</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="G32" t="s">
         <v>18</v>
       </c>
       <c r="H32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D33" s="2">
-        <v>45091.583333333343</v>
+        <v>44946.489583333343</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H33" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="2">
-        <v>45096.6875</v>
+        <v>45261.385416666657</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="G34" t="s">
         <v>18</v>
       </c>
       <c r="H34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D35" s="2">
-        <v>45101.385416666657</v>
+        <v>45016.385416666657</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="G35" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D36" s="2">
-        <v>45106.458333333343</v>
+        <v>45176.583333333343</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G36" t="s">
         <v>18</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D37" s="2">
-        <v>45111.572916666657</v>
+        <v>45331.458333333343</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D38" s="2">
-        <v>45116.645833333343</v>
+        <v>44977.645833333343</v>
       </c>
       <c r="E38" t="s">
         <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="G38" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D39" s="2">
-        <v>45121.375</v>
+        <v>45131.489583333343</v>
       </c>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="G39" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H39" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D40" s="2">
-        <v>45126.677083333343</v>
+        <v>45281.385416666657</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="G40" t="s">
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="2">
-        <v>45131.489583333343</v>
+        <v>44996.53125</v>
       </c>
       <c r="E41" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="G41" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D42" s="2">
-        <v>45136.583333333343</v>
+        <v>45111.572916666657</v>
       </c>
       <c r="E42" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="G42" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H42" t="s">
         <v>19</v>
@@ -1755,94 +1765,94 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D43" s="2">
-        <v>45141.385416666657</v>
+        <v>45271.489583333343</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="2">
-        <v>45146.458333333343</v>
+        <v>45026.572916666657</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="G44" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="2">
-        <v>45151.572916666657</v>
+        <v>45181.385416666657</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="G45" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D46" s="2">
-        <v>45156.645833333343</v>
+        <v>45341.645833333343</v>
       </c>
       <c r="E46" t="s">
         <v>40</v>
@@ -1854,264 +1864,264 @@
         <v>18</v>
       </c>
       <c r="H46" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D47" s="2">
-        <v>45161.375</v>
+        <v>45091.583333333343</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="F47" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="G47" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="2">
-        <v>45166.677083333343</v>
+        <v>45196.645833333343</v>
       </c>
       <c r="E48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F48" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="G48" t="s">
         <v>18</v>
       </c>
       <c r="H48" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="2">
-        <v>45171.489583333343</v>
+        <v>45036.375</v>
       </c>
       <c r="E49" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="F49" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G49" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H49" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="2">
-        <v>45176.583333333343</v>
+        <v>45161.375</v>
       </c>
       <c r="E50" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="F50" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="G50" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H50" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="2">
-        <v>45181.385416666657</v>
+        <v>45301.375</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="F51" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H51" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="2">
+        <v>44967.40625</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
         <v>32</v>
       </c>
-      <c r="B52" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="2">
-        <v>45186.458333333343</v>
-      </c>
-      <c r="E52" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" t="s">
-        <v>44</v>
-      </c>
       <c r="G52" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D53" s="2">
-        <v>45191.572916666657</v>
+        <v>45126.677083333343</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="F53" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="G53" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H53" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
       <c r="D54" s="2">
-        <v>45196.645833333343</v>
+        <v>45361.583333333343</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F54" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="G54" t="s">
         <v>18</v>
       </c>
       <c r="H54" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D55" s="2">
-        <v>45201.375</v>
+        <v>44956.427083333343</v>
       </c>
       <c r="E55" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D56" s="2">
-        <v>45206.677083333343</v>
+        <v>45156.645833333343</v>
       </c>
       <c r="E56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F56" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H56" t="s">
         <v>13</v>
@@ -2119,207 +2129,207 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D57" s="2">
-        <v>45211.489583333343</v>
+        <v>45251.489583333343</v>
       </c>
       <c r="E57" t="s">
         <v>22</v>
       </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="G57" t="s">
         <v>18</v>
       </c>
       <c r="H57" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D58" s="2">
-        <v>45216.583333333343</v>
+        <v>45046.489583333343</v>
       </c>
       <c r="E58" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="G58" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H58" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="2">
-        <v>45221.385416666657</v>
+        <v>45326.6875</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G59" t="s">
         <v>18</v>
       </c>
       <c r="H59" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D60" s="2">
-        <v>45226.458333333343</v>
+        <v>45041.677083333343</v>
       </c>
       <c r="E60" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F60" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G60" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H60" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D61" s="2">
-        <v>45231.572916666657</v>
+        <v>45191.572916666657</v>
       </c>
       <c r="E61" t="s">
         <v>61</v>
       </c>
       <c r="F61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G61" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H61" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D62" s="2">
-        <v>45236.645833333343</v>
+        <v>45291.572916666657</v>
       </c>
       <c r="E62" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="G62" t="s">
         <v>18</v>
       </c>
       <c r="H62" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D63" s="2">
-        <v>45241.375</v>
+        <v>45071.541666666657</v>
       </c>
       <c r="E63" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="F63" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="G63" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H63" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
         <v>21</v>
       </c>
       <c r="D64" s="2">
-        <v>45246.677083333343</v>
+        <v>45021.458333333343</v>
       </c>
       <c r="E64" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="G64" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H64" t="s">
         <v>25</v>
@@ -2327,201 +2337,201 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="2">
-        <v>45251.489583333343</v>
+        <v>45116.645833333343</v>
       </c>
       <c r="E65" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F65" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="G65" t="s">
         <v>18</v>
       </c>
       <c r="H65" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D66" s="2">
-        <v>45256.583333333343</v>
+        <v>45321.385416666657</v>
       </c>
       <c r="E66" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F66" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H66" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="2">
-        <v>45261.385416666657</v>
+        <v>45081.375</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="F67" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G67" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H67" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
       </c>
       <c r="D68" s="2">
-        <v>45266.6875</v>
+        <v>45221.385416666657</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G68" t="s">
         <v>18</v>
       </c>
       <c r="H68" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
       </c>
       <c r="D69" s="2">
-        <v>45271.489583333343</v>
+        <v>45076.65625</v>
       </c>
       <c r="E69" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="F69" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G69" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H69" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
       </c>
       <c r="D70" s="2">
-        <v>45276.583333333343</v>
+        <v>45231.572916666657</v>
       </c>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F70" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G70" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H70" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D71" s="2">
-        <v>45281.385416666657</v>
+        <v>45366.385416666657</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="G71" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H71" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D72" s="2">
-        <v>45286.458333333343</v>
+        <v>45086.46875</v>
       </c>
       <c r="E72" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="F72" t="s">
         <v>22</v>
@@ -2535,77 +2545,77 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D73" s="2">
-        <v>45291.572916666657</v>
+        <v>45226.458333333343</v>
       </c>
       <c r="E73" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="G73" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H73" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D74" s="2">
-        <v>45296.645833333343</v>
+        <v>45316.583333333343</v>
       </c>
       <c r="E74" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F74" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G74" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H74" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="2">
-        <v>45301.375</v>
+        <v>45001.583333333343</v>
       </c>
       <c r="E75" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="F75" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G75" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H75" t="s">
         <v>30</v>
@@ -2613,230 +2623,230 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C76" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D76" s="2">
-        <v>45306.677083333343</v>
+        <v>45136.583333333343</v>
       </c>
       <c r="E76" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F76" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="G76" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H76" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D77" s="2">
-        <v>45311.489583333343</v>
+        <v>45351.677083333343</v>
       </c>
       <c r="E77" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F77" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="G77" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H77" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D78" s="2">
-        <v>45316.583333333343</v>
+        <v>44982.458333333343</v>
       </c>
       <c r="E78" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="G78" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H78" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D79" s="2">
-        <v>45321.385416666657</v>
+        <v>45206.677083333343</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F79" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="G79" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H79" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D80" s="2">
-        <v>45326.6875</v>
+        <v>45066.427083333343</v>
       </c>
       <c r="E80" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F80" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="G80" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H80" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D81" s="2">
-        <v>45331.458333333343</v>
+        <v>45216.583333333343</v>
       </c>
       <c r="E81" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F81" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="G81" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H81" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C82" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D82" s="2">
-        <v>45336.572916666657</v>
+        <v>45346.375</v>
       </c>
       <c r="E82" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F82" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="G82" t="s">
         <v>18</v>
       </c>
       <c r="H82" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D83" s="2">
-        <v>45341.645833333343</v>
+        <v>45006.4375</v>
       </c>
       <c r="E83" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F83" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G83" t="s">
         <v>18</v>
       </c>
       <c r="H83" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C84" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D84" s="2">
-        <v>45346.375</v>
+        <v>45371.6875</v>
       </c>
       <c r="E84" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="F84" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="G84" t="s">
         <v>18</v>
@@ -2847,74 +2857,74 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="C85" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D85" s="2">
-        <v>45351.677083333343</v>
+        <v>45061.697916666657</v>
       </c>
       <c r="E85" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F85" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="G85" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H85" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D86" s="2">
-        <v>45356.489583333343</v>
+        <v>45186.458333333343</v>
       </c>
       <c r="E86" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="G86" t="s">
         <v>18</v>
       </c>
       <c r="H86" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C87" t="s">
         <v>15</v>
       </c>
       <c r="D87" s="2">
-        <v>45361.583333333343</v>
+        <v>45286.458333333343</v>
       </c>
       <c r="E87" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="G87" t="s">
         <v>18</v>
@@ -2925,57 +2935,62 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C88" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D88" s="2">
-        <v>45366.385416666657</v>
+        <v>45031.645833333343</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F88" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G88" t="s">
         <v>18</v>
       </c>
       <c r="H88" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C89" t="s">
         <v>9</v>
       </c>
       <c r="D89" s="2">
-        <v>45371.6875</v>
+        <v>45356.489583333343</v>
       </c>
       <c r="E89" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F89" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="G89" t="s">
         <v>18</v>
       </c>
       <c r="H89" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H89" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H89">
+      <sortCondition ref="A1:A89"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>